<commit_message>
push result datasheet and upset diagram for 3 dataset and simple motivation example
</commit_message>
<xml_diff>
--- a/training-data/result-sheet/106-dataset/raw_strata_fix_rate.xlsx
+++ b/training-data/result-sheet/106-dataset/raw_strata_fix_rate.xlsx
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>457</v>
+        <v>267</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -483,10 +483,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -502,19 +502,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>459</v>
+        <v>262</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -533,19 +533,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" t="n">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -564,10 +564,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C5" t="n">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D5" t="n">
         <v>2</v>
@@ -576,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -595,22 +595,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C6" t="n">
-        <v>397</v>
+        <v>252</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C7" t="n">
-        <v>392</v>
+        <v>246</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -657,19 +657,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -688,10 +688,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C9" t="n">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -719,19 +719,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C10" t="n">
-        <v>426</v>
+        <v>248</v>
       </c>
       <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
         <v>6</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>18</v>
       </c>
       <c r="G10" t="n">
         <v>3</v>
@@ -750,22 +750,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="C11" t="n">
-        <v>388</v>
+        <v>226</v>
       </c>
       <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
         <v>4</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>10</v>
-      </c>
       <c r="G11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -781,19 +781,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C12" t="n">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -812,19 +812,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C13" t="n">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -843,22 +843,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C14" t="n">
-        <v>364</v>
+        <v>234</v>
       </c>
       <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8</v>
+      </c>
+      <c r="G14" t="n">
         <v>6</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>17</v>
-      </c>
-      <c r="G14" t="n">
-        <v>10</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -874,22 +874,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="C15" t="n">
-        <v>327</v>
+        <v>213</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G15" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -905,22 +905,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C16" t="n">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G16" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
@@ -936,22 +936,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C17" t="n">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>11</v>
+      </c>
+      <c r="G17" t="n">
         <v>7</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>16</v>
-      </c>
-      <c r="G17" t="n">
-        <v>3</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -967,10 +967,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>483</v>
+        <v>276</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -979,10 +979,10 @@
         <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>1</v>
@@ -998,19 +998,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C19" t="n">
-        <v>483</v>
+        <v>272</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1029,10 +1029,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C20" t="n">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G20" t="n">
         <v>2</v>
@@ -1060,10 +1060,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C21" t="n">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D21" t="n">
         <v>1</v>
@@ -1072,10 +1072,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1091,19 +1091,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C22" t="n">
-        <v>426</v>
+        <v>265</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G22" t="n">
         <v>1</v>
@@ -1122,10 +1122,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C23" t="n">
-        <v>404</v>
+        <v>256</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -1134,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1153,10 +1153,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C24" t="n">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1165,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1184,10 +1184,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C25" t="n">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -1215,19 +1215,19 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C26" t="n">
-        <v>436</v>
+        <v>251</v>
       </c>
       <c r="D26" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -1246,19 +1246,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="C27" t="n">
-        <v>389</v>
+        <v>225</v>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -1277,19 +1277,19 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C28" t="n">
         <v>234</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G28" t="n">
         <v>1</v>
@@ -1308,19 +1308,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C29" t="n">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
         <v>6</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
-        <v>12</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1339,22 +1339,22 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="C30" t="n">
-        <v>366</v>
+        <v>227</v>
       </c>
       <c r="D30" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G30" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1370,22 +1370,22 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>128</v>
+        <v>67</v>
       </c>
       <c r="C31" t="n">
-        <v>322</v>
+        <v>218</v>
       </c>
       <c r="D31" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
         <v>6</v>
       </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>15</v>
-      </c>
       <c r="G31" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1401,22 +1401,22 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C32" t="n">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G32" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1432,22 +1432,22 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C33" t="n">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D33" t="n">
+        <v>3</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>8</v>
+      </c>
+      <c r="G33" t="n">
         <v>6</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>14</v>
-      </c>
-      <c r="G33" t="n">
-        <v>3</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1463,10 +1463,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" t="n">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G34" t="n">
         <v>3</v>
@@ -1494,19 +1494,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C35" t="n">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G35" t="n">
         <v>2</v>
@@ -1525,22 +1525,22 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C36" t="n">
-        <v>117</v>
+        <v>237</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G36" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1556,10 +1556,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C37" t="n">
-        <v>111</v>
+        <v>233</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -1568,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -1587,22 +1587,22 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C38" t="n">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G38" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1618,19 +1618,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -1649,22 +1649,22 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C40" t="n">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -1680,10 +1680,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="C41" t="n">
-        <v>97</v>
+        <v>215</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
@@ -1711,19 +1711,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C42" t="n">
-        <v>205</v>
+        <v>233</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G42" t="n">
         <v>2</v>
@@ -1742,22 +1742,22 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C43" t="n">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -1773,19 +1773,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C44" t="n">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E44" t="n">
         <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G44" t="n">
         <v>2</v>
@@ -1804,22 +1804,22 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="C45" t="n">
-        <v>98</v>
+        <v>197</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
+        <v>10</v>
+      </c>
+      <c r="G45" t="n">
         <v>2</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -1835,22 +1835,22 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C46" t="n">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G46" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -1866,22 +1866,22 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C47" t="n">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G47" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -1897,22 +1897,22 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C48" t="n">
-        <v>100</v>
+        <v>218</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G48" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H48" t="n">
         <v>1</v>
@@ -1928,22 +1928,22 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="C49" t="n">
-        <v>93</v>
+        <v>198</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G49" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -1962,7 +1962,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="n">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -1971,10 +1971,10 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G50" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -1990,19 +1990,19 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C51" t="n">
-        <v>235</v>
+        <v>279</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G51" t="n">
         <v>1</v>
@@ -2021,10 +2021,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>112</v>
+        <v>241</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G52" t="n">
         <v>1</v>
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C53" t="n">
-        <v>103</v>
+        <v>226</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
@@ -2064,10 +2064,10 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2083,19 +2083,19 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C54" t="n">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
@@ -2114,10 +2114,10 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C55" t="n">
-        <v>212</v>
+        <v>257</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G55" t="n">
         <v>0</v>
@@ -2145,10 +2145,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C56" t="n">
-        <v>105</v>
+        <v>239</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G56" t="n">
         <v>2</v>
@@ -2176,10 +2176,10 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C57" t="n">
-        <v>99</v>
+        <v>221</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
@@ -2188,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
@@ -2207,22 +2207,22 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C58" t="n">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2238,19 +2238,19 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C59" t="n">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -2269,22 +2269,22 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>119</v>
+        <v>232</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -2300,19 +2300,19 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C61" t="n">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
@@ -2331,22 +2331,22 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C62" t="n">
-        <v>189</v>
+        <v>232</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G62" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2362,22 +2362,22 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C63" t="n">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G63" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2393,22 +2393,22 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C64" t="n">
-        <v>101</v>
+        <v>222</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G64" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -2424,22 +2424,22 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="C65" t="n">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G65" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>

</xml_diff>